<commit_message>
feuille de route mise à jour
</commit_message>
<xml_diff>
--- a/assets/Feuille_de_route.xlsx
+++ b/assets/Feuille_de_route.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{649A8032-70AE-4EF8-A3BB-44A30EDFE42A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{C7AA8CE3-34D1-4224-B767-C2AA1FDA7D4F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>Ville - Entreprise</t>
   </si>
@@ -83,6 +83,12 @@
   </si>
   <si>
     <t>Volvo FH Globetrotter</t>
+  </si>
+  <si>
+    <t>Divers</t>
+  </si>
+  <si>
+    <t>Distance parcourue</t>
   </si>
 </sst>
 </file>
@@ -143,7 +149,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -462,43 +468,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -558,6 +527,28 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -569,7 +560,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -649,154 +640,172 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="33" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1118,10 +1127,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:M37"/>
+  <dimension ref="B1:N37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34:K34"/>
+      <selection activeCell="B2" sqref="B2:M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1137,41 +1146,44 @@
     <col min="9" max="9" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15" style="1" customWidth="1"/>
-    <col min="12" max="12" width="38.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="1.7109375" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="11.42578125" style="1"/>
+    <col min="12" max="12" width="19.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="38.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="1.7109375" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="50" t="s">
+    <row r="1" spans="2:14" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="52"/>
-    </row>
-    <row r="3" spans="2:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="53"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="55"/>
-    </row>
-    <row r="4" spans="2:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="51"/>
+    </row>
+    <row r="3" spans="2:14" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="52"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="54"/>
+    </row>
+    <row r="4" spans="2:14" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -1183,68 +1195,70 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
-    </row>
-    <row r="5" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E5" s="56" t="s">
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="66" t="s">
+      <c r="F5" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="67"/>
-      <c r="H5" s="68" t="s">
+      <c r="G5" s="64"/>
+      <c r="H5" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="69"/>
-    </row>
-    <row r="6" spans="2:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E6" s="57"/>
+      <c r="I5" s="66"/>
+    </row>
+    <row r="6" spans="2:14" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E6" s="56"/>
       <c r="F6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="70"/>
-      <c r="I6" s="71"/>
-    </row>
-    <row r="7" spans="2:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H6" s="67"/>
+      <c r="I6" s="68"/>
+    </row>
+    <row r="7" spans="2:14" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E7" s="4" t="s">
         <v>18</v>
       </c>
       <c r="F7" s="24"/>
       <c r="G7" s="25"/>
-      <c r="H7" s="72" t="s">
+      <c r="H7" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="62"/>
-    </row>
-    <row r="8" spans="2:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="2:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="61" t="s">
+      <c r="I7" s="61"/>
+    </row>
+    <row r="8" spans="2:14" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="2:14" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="62"/>
-      <c r="D9" s="61" t="s">
+      <c r="C9" s="61"/>
+      <c r="D9" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="62"/>
-      <c r="F9" s="61" t="s">
+      <c r="E9" s="61"/>
+      <c r="F9" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="63"/>
-      <c r="H9" s="62"/>
-      <c r="I9" s="61" t="s">
+      <c r="G9" s="62"/>
+      <c r="H9" s="61"/>
+      <c r="I9" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="63"/>
-      <c r="K9" s="62"/>
-      <c r="L9" s="64" t="s">
-        <v>17</v>
-      </c>
-      <c r="M9" s="26"/>
-    </row>
-    <row r="10" spans="2:13" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J9" s="62"/>
+      <c r="K9" s="61"/>
+      <c r="L9" s="60" t="s">
+        <v>21</v>
+      </c>
+      <c r="M9" s="61"/>
+      <c r="N9" s="26"/>
+    </row>
+    <row r="10" spans="2:14" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
         <v>1</v>
       </c>
@@ -1275,348 +1289,378 @@
       <c r="K10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="L10" s="65"/>
-      <c r="M10" s="26"/>
-    </row>
-    <row r="11" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L10" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="M10" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="N10" s="26"/>
+    </row>
+    <row r="11" spans="2:14" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="9"/>
       <c r="C11" s="10"/>
       <c r="D11" s="11"/>
       <c r="E11" s="10"/>
       <c r="F11" s="12"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="37"/>
-      <c r="K11" s="36"/>
-      <c r="L11" s="30"/>
-    </row>
-    <row r="12" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G11" s="27"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="78"/>
+      <c r="M11" s="75"/>
+    </row>
+    <row r="12" spans="2:14" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="13"/>
       <c r="C12" s="14"/>
       <c r="D12" s="15"/>
       <c r="E12" s="14"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="40"/>
-      <c r="K12" s="39"/>
-      <c r="L12" s="27"/>
-    </row>
-    <row r="13" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G12" s="28"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="35"/>
+      <c r="L12" s="79"/>
+      <c r="M12" s="74"/>
+    </row>
+    <row r="13" spans="2:14" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="16"/>
       <c r="C13" s="17"/>
       <c r="D13" s="18"/>
       <c r="E13" s="17"/>
       <c r="F13" s="19"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="42"/>
-      <c r="L13" s="28"/>
-    </row>
-    <row r="14" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G13" s="29"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="38"/>
+      <c r="L13" s="80"/>
+      <c r="M13" s="76"/>
+    </row>
+    <row r="14" spans="2:14" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="13"/>
       <c r="C14" s="14"/>
       <c r="D14" s="15"/>
       <c r="E14" s="14"/>
       <c r="F14" s="6"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="40"/>
-      <c r="K14" s="39"/>
-      <c r="L14" s="27"/>
-    </row>
-    <row r="15" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G14" s="28"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="36"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="79"/>
+      <c r="M14" s="74"/>
+    </row>
+    <row r="15" spans="2:14" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="16"/>
       <c r="C15" s="17"/>
       <c r="D15" s="18"/>
       <c r="E15" s="17"/>
       <c r="F15" s="19"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="42"/>
-      <c r="J15" s="43"/>
-      <c r="K15" s="42"/>
-      <c r="L15" s="28"/>
-    </row>
-    <row r="16" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G15" s="29"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="80"/>
+      <c r="M15" s="76"/>
+    </row>
+    <row r="16" spans="2:14" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="13"/>
       <c r="C16" s="14"/>
       <c r="D16" s="15"/>
       <c r="E16" s="14"/>
       <c r="F16" s="6"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="40"/>
-      <c r="K16" s="39"/>
-      <c r="L16" s="27"/>
-    </row>
-    <row r="17" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G16" s="28"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="36"/>
+      <c r="K16" s="35"/>
+      <c r="L16" s="79"/>
+      <c r="M16" s="74"/>
+    </row>
+    <row r="17" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="16"/>
       <c r="C17" s="17"/>
       <c r="D17" s="18"/>
       <c r="E17" s="17"/>
       <c r="F17" s="19"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="43"/>
-      <c r="K17" s="42"/>
-      <c r="L17" s="28"/>
-    </row>
-    <row r="18" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G17" s="29"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="38"/>
+      <c r="L17" s="80"/>
+      <c r="M17" s="76"/>
+    </row>
+    <row r="18" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="13"/>
       <c r="C18" s="14"/>
       <c r="D18" s="15"/>
       <c r="E18" s="14"/>
       <c r="F18" s="6"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="40"/>
-      <c r="K18" s="39"/>
-      <c r="L18" s="27"/>
-    </row>
-    <row r="19" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G18" s="28"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="36"/>
+      <c r="K18" s="35"/>
+      <c r="L18" s="79"/>
+      <c r="M18" s="74"/>
+    </row>
+    <row r="19" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="16"/>
       <c r="C19" s="17"/>
       <c r="D19" s="18"/>
       <c r="E19" s="17"/>
       <c r="F19" s="19"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="42"/>
-      <c r="J19" s="43"/>
-      <c r="K19" s="42"/>
-      <c r="L19" s="28"/>
-    </row>
-    <row r="20" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G19" s="29"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="80"/>
+      <c r="M19" s="76"/>
+    </row>
+    <row r="20" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="13"/>
       <c r="C20" s="14"/>
       <c r="D20" s="15"/>
       <c r="E20" s="14"/>
       <c r="F20" s="6"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="40"/>
-      <c r="K20" s="39"/>
-      <c r="L20" s="27"/>
-    </row>
-    <row r="21" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G20" s="28"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="35"/>
+      <c r="J20" s="36"/>
+      <c r="K20" s="35"/>
+      <c r="L20" s="79"/>
+      <c r="M20" s="74"/>
+    </row>
+    <row r="21" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="16"/>
       <c r="C21" s="17"/>
       <c r="D21" s="18"/>
       <c r="E21" s="17"/>
       <c r="F21" s="19"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="41"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="43"/>
-      <c r="K21" s="42"/>
-      <c r="L21" s="28"/>
-    </row>
-    <row r="22" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G21" s="29"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="38"/>
+      <c r="L21" s="80"/>
+      <c r="M21" s="76"/>
+    </row>
+    <row r="22" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="13"/>
       <c r="C22" s="14"/>
       <c r="D22" s="15"/>
       <c r="E22" s="14"/>
       <c r="F22" s="6"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="40"/>
-      <c r="K22" s="39"/>
-      <c r="L22" s="27"/>
-    </row>
-    <row r="23" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G22" s="28"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="35"/>
+      <c r="J22" s="36"/>
+      <c r="K22" s="35"/>
+      <c r="L22" s="79"/>
+      <c r="M22" s="74"/>
+    </row>
+    <row r="23" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="16"/>
       <c r="C23" s="17"/>
       <c r="D23" s="18"/>
       <c r="E23" s="17"/>
       <c r="F23" s="19"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="41"/>
-      <c r="I23" s="42"/>
-      <c r="J23" s="43"/>
-      <c r="K23" s="42"/>
-      <c r="L23" s="28"/>
-    </row>
-    <row r="24" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G23" s="29"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="38"/>
+      <c r="L23" s="80"/>
+      <c r="M23" s="76"/>
+    </row>
+    <row r="24" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="13"/>
       <c r="C24" s="14"/>
       <c r="D24" s="15"/>
       <c r="E24" s="14"/>
       <c r="F24" s="6"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="39"/>
-      <c r="J24" s="40"/>
-      <c r="K24" s="39"/>
-      <c r="L24" s="27"/>
-    </row>
-    <row r="25" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G24" s="28"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="35"/>
+      <c r="L24" s="79"/>
+      <c r="M24" s="74"/>
+    </row>
+    <row r="25" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="16"/>
       <c r="C25" s="17"/>
       <c r="D25" s="18"/>
       <c r="E25" s="17"/>
       <c r="F25" s="19"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="41"/>
-      <c r="I25" s="42"/>
-      <c r="J25" s="43"/>
-      <c r="K25" s="42"/>
-      <c r="L25" s="28"/>
-    </row>
-    <row r="26" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G25" s="29"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="38"/>
+      <c r="J25" s="39"/>
+      <c r="K25" s="38"/>
+      <c r="L25" s="80"/>
+      <c r="M25" s="76"/>
+    </row>
+    <row r="26" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="13"/>
       <c r="C26" s="14"/>
       <c r="D26" s="15"/>
       <c r="E26" s="14"/>
       <c r="F26" s="6"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="38"/>
-      <c r="I26" s="39"/>
-      <c r="J26" s="40"/>
-      <c r="K26" s="39"/>
-      <c r="L26" s="27"/>
-    </row>
-    <row r="27" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G26" s="28"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="35"/>
+      <c r="J26" s="36"/>
+      <c r="K26" s="35"/>
+      <c r="L26" s="79"/>
+      <c r="M26" s="74"/>
+    </row>
+    <row r="27" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="16"/>
       <c r="C27" s="17"/>
       <c r="D27" s="18"/>
       <c r="E27" s="17"/>
       <c r="F27" s="19"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="41"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="43"/>
-      <c r="K27" s="42"/>
-      <c r="L27" s="28"/>
-    </row>
-    <row r="28" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G27" s="29"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="39"/>
+      <c r="K27" s="38"/>
+      <c r="L27" s="80"/>
+      <c r="M27" s="76"/>
+    </row>
+    <row r="28" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="20"/>
       <c r="C28" s="21"/>
       <c r="D28" s="22"/>
       <c r="E28" s="21"/>
       <c r="F28" s="23"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="44"/>
-      <c r="I28" s="45"/>
-      <c r="J28" s="46"/>
-      <c r="K28" s="45"/>
-      <c r="L28" s="29"/>
-    </row>
-    <row r="29" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G28" s="30"/>
+      <c r="H28" s="40"/>
+      <c r="I28" s="41"/>
+      <c r="J28" s="42"/>
+      <c r="K28" s="41"/>
+      <c r="L28" s="81"/>
+      <c r="M28" s="77"/>
+    </row>
+    <row r="29" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="16"/>
       <c r="C29" s="17"/>
       <c r="D29" s="18"/>
       <c r="E29" s="17"/>
       <c r="F29" s="19"/>
-      <c r="G29" s="33"/>
-      <c r="H29" s="41"/>
-      <c r="I29" s="42"/>
-      <c r="J29" s="43"/>
-      <c r="K29" s="42"/>
-      <c r="L29" s="28"/>
-    </row>
-    <row r="30" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G29" s="29"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="38"/>
+      <c r="L29" s="80"/>
+      <c r="M29" s="76"/>
+    </row>
+    <row r="30" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="13"/>
       <c r="C30" s="14"/>
       <c r="D30" s="15"/>
       <c r="E30" s="14"/>
       <c r="F30" s="6"/>
-      <c r="G30" s="32"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="39"/>
-      <c r="J30" s="40"/>
-      <c r="K30" s="39"/>
-      <c r="L30" s="27"/>
-    </row>
-    <row r="31" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G30" s="28"/>
+      <c r="H30" s="34"/>
+      <c r="I30" s="35"/>
+      <c r="J30" s="36"/>
+      <c r="K30" s="35"/>
+      <c r="L30" s="79"/>
+      <c r="M30" s="74"/>
+    </row>
+    <row r="31" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="16"/>
       <c r="C31" s="17"/>
       <c r="D31" s="18"/>
       <c r="E31" s="17"/>
       <c r="F31" s="19"/>
-      <c r="G31" s="33"/>
-      <c r="H31" s="41"/>
-      <c r="I31" s="42"/>
-      <c r="J31" s="43"/>
-      <c r="K31" s="42"/>
-      <c r="L31" s="28"/>
-    </row>
-    <row r="32" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G31" s="29"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="39"/>
+      <c r="K31" s="38"/>
+      <c r="L31" s="80"/>
+      <c r="M31" s="76"/>
+    </row>
+    <row r="32" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="13"/>
       <c r="C32" s="14"/>
       <c r="D32" s="15"/>
       <c r="E32" s="14"/>
       <c r="F32" s="6"/>
-      <c r="G32" s="32"/>
-      <c r="H32" s="38"/>
-      <c r="I32" s="39"/>
-      <c r="J32" s="40"/>
-      <c r="K32" s="39"/>
-      <c r="L32" s="27"/>
-    </row>
-    <row r="33" spans="2:12" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G32" s="28"/>
+      <c r="H32" s="34"/>
+      <c r="I32" s="35"/>
+      <c r="J32" s="36"/>
+      <c r="K32" s="35"/>
+      <c r="L32" s="79"/>
+      <c r="M32" s="74"/>
+    </row>
+    <row r="33" spans="2:13" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="16"/>
       <c r="C33" s="17"/>
       <c r="D33" s="18"/>
       <c r="E33" s="17"/>
       <c r="F33" s="19"/>
-      <c r="G33" s="33"/>
-      <c r="H33" s="41"/>
-      <c r="I33" s="42"/>
-      <c r="J33" s="43"/>
-      <c r="K33" s="42"/>
-      <c r="L33" s="28"/>
-    </row>
-    <row r="34" spans="2:12" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="61" t="s">
+      <c r="G33" s="29"/>
+      <c r="H33" s="37"/>
+      <c r="I33" s="38"/>
+      <c r="J33" s="39"/>
+      <c r="K33" s="38"/>
+      <c r="L33" s="82"/>
+      <c r="M33" s="76"/>
+    </row>
+    <row r="34" spans="2:13" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="C34" s="63"/>
-      <c r="D34" s="63"/>
-      <c r="E34" s="63"/>
-      <c r="F34" s="73"/>
-      <c r="G34" s="47">
+      <c r="C34" s="62"/>
+      <c r="D34" s="62"/>
+      <c r="E34" s="62"/>
+      <c r="F34" s="70"/>
+      <c r="G34" s="43">
         <f>SUM(G11:G33)</f>
         <v>0</v>
       </c>
-      <c r="H34" s="48">
-        <f t="shared" ref="H34:K34" si="0">SUM(H11:H33)</f>
+      <c r="H34" s="44">
+        <f t="shared" ref="H34" si="0">SUM(H11:H33)</f>
         <v>0</v>
       </c>
-      <c r="I34" s="74">
+      <c r="I34" s="71">
         <f>SUM(I11:K33)</f>
         <v>0</v>
       </c>
-      <c r="J34" s="75"/>
-      <c r="K34" s="76"/>
-      <c r="L34" s="49"/>
-    </row>
-    <row r="35" spans="2:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="36" spans="2:12" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E36" s="58" t="s">
+      <c r="J34" s="72"/>
+      <c r="K34" s="73"/>
+      <c r="L34" s="48"/>
+      <c r="M34" s="45"/>
+    </row>
+    <row r="35" spans="2:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="2:13" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E36" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="F36" s="59"/>
-      <c r="G36" s="59"/>
-      <c r="H36" s="59"/>
-      <c r="I36" s="59"/>
-      <c r="J36" s="60"/>
+      <c r="F36" s="58"/>
+      <c r="G36" s="58"/>
+      <c r="H36" s="58"/>
+      <c r="I36" s="58"/>
+      <c r="J36" s="59"/>
       <c r="K36" s="6"/>
-    </row>
-    <row r="37" spans="2:12" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="L36" s="6"/>
+    </row>
+    <row r="37" spans="2:13" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B2:L3"/>
+    <mergeCell ref="B2:M3"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="E36:G36"/>
     <mergeCell ref="H36:J36"/>
@@ -1624,12 +1668,12 @@
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="F9:H9"/>
     <mergeCell ref="I9:K9"/>
-    <mergeCell ref="L9:L10"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="H5:I6"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="B34:F34"/>
     <mergeCell ref="I34:K34"/>
+    <mergeCell ref="L9:M9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="287" scale="59" orientation="landscape" r:id="rId1"/>

</xml_diff>